<commit_message>
nuevo datos y archvios de busqueda de parametros
</commit_message>
<xml_diff>
--- a/resultados_parametros_optimization.xlsx
+++ b/resultados_parametros_optimization.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X262"/>
+  <dimension ref="A1:X282"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -22637,10 +22637,8 @@
       <c r="C253" t="n">
         <v>10</v>
       </c>
-      <c r="D253" t="inlineStr">
-        <is>
-          <t>146</t>
-        </is>
+      <c r="D253" t="n">
+        <v>146</v>
       </c>
       <c r="E253" t="n">
         <v>0.04972875118255615</v>
@@ -22727,10 +22725,8 @@
       <c r="C254" t="n">
         <v>10</v>
       </c>
-      <c r="D254" t="inlineStr">
-        <is>
-          <t>019</t>
-        </is>
+      <c r="D254" t="n">
+        <v>19</v>
       </c>
       <c r="E254" t="n">
         <v>0.04520795494318008</v>
@@ -22817,10 +22813,8 @@
       <c r="C255" t="n">
         <v>10</v>
       </c>
-      <c r="D255" t="inlineStr">
-        <is>
-          <t>106</t>
-        </is>
+      <c r="D255" t="n">
+        <v>106</v>
       </c>
       <c r="E255" t="n">
         <v>0.04520795494318008</v>
@@ -22907,10 +22901,8 @@
       <c r="C256" t="n">
         <v>10</v>
       </c>
-      <c r="D256" t="inlineStr">
-        <is>
-          <t>011</t>
-        </is>
+      <c r="D256" t="n">
+        <v>11</v>
       </c>
       <c r="E256" t="n">
         <v>0.04430379718542099</v>
@@ -22997,10 +22989,8 @@
       <c r="C257" t="n">
         <v>10</v>
       </c>
-      <c r="D257" t="inlineStr">
-        <is>
-          <t>201</t>
-        </is>
+      <c r="D257" t="n">
+        <v>201</v>
       </c>
       <c r="E257" t="n">
         <v>0.04430379718542099</v>
@@ -23087,10 +23077,8 @@
       <c r="C258" t="n">
         <v>10</v>
       </c>
-      <c r="D258" t="inlineStr">
-        <is>
-          <t>298</t>
-        </is>
+      <c r="D258" t="n">
+        <v>298</v>
       </c>
       <c r="E258" t="n">
         <v>0.04430379718542099</v>
@@ -23177,10 +23165,8 @@
       <c r="C259" t="n">
         <v>10</v>
       </c>
-      <c r="D259" t="inlineStr">
-        <is>
-          <t>014</t>
-        </is>
+      <c r="D259" t="n">
+        <v>14</v>
       </c>
       <c r="E259" t="n">
         <v>0.0433996394276619</v>
@@ -23267,10 +23253,8 @@
       <c r="C260" t="n">
         <v>10</v>
       </c>
-      <c r="D260" t="inlineStr">
-        <is>
-          <t>038</t>
-        </is>
+      <c r="D260" t="n">
+        <v>38</v>
       </c>
       <c r="E260" t="n">
         <v>0.0433996394276619</v>
@@ -23357,10 +23341,8 @@
       <c r="C261" t="n">
         <v>10</v>
       </c>
-      <c r="D261" t="inlineStr">
-        <is>
-          <t>042</t>
-        </is>
+      <c r="D261" t="n">
+        <v>42</v>
       </c>
       <c r="E261" t="n">
         <v>0.0433996394276619</v>
@@ -23447,10 +23429,8 @@
       <c r="C262" t="n">
         <v>10</v>
       </c>
-      <c r="D262" t="inlineStr">
-        <is>
-          <t>077</t>
-        </is>
+      <c r="D262" t="n">
+        <v>77</v>
       </c>
       <c r="E262" t="n">
         <v>0.0433996394276619</v>
@@ -23523,6 +23503,1786 @@
       </c>
       <c r="X262" t="n">
         <v>64</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>bayesian_optimization</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>50</v>
+      </c>
+      <c r="C263" t="n">
+        <v>6</v>
+      </c>
+      <c r="D263" t="n">
+        <v>84</v>
+      </c>
+      <c r="E263" t="n">
+        <v>0.0496838316321373</v>
+      </c>
+      <c r="F263" t="n">
+        <v>0.0496838316321373</v>
+      </c>
+      <c r="G263" t="n">
+        <v>4.303908348083496</v>
+      </c>
+      <c r="H263" t="n">
+        <v>0.00223370257188463</v>
+      </c>
+      <c r="I263" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="J263" t="n">
+        <v>0.001559041244007198</v>
+      </c>
+      <c r="K263" t="n">
+        <v>56</v>
+      </c>
+      <c r="L263" t="n">
+        <v>64</v>
+      </c>
+      <c r="M263" t="n">
+        <v>256</v>
+      </c>
+      <c r="N263" t="n">
+        <v>128</v>
+      </c>
+      <c r="O263" t="n">
+        <v>32</v>
+      </c>
+      <c r="P263" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q263" t="n">
+        <v>2</v>
+      </c>
+      <c r="R263" t="inlineStr">
+        <is>
+          <t>rmsprop</t>
+        </is>
+      </c>
+      <c r="S263" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="T263" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U263" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="V263" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="W263" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="X263" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>bayesian_optimization</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>50</v>
+      </c>
+      <c r="C264" t="n">
+        <v>6</v>
+      </c>
+      <c r="D264" t="n">
+        <v>142</v>
+      </c>
+      <c r="E264" t="n">
+        <v>0.0496838316321373</v>
+      </c>
+      <c r="F264" t="n">
+        <v>0.0496838316321373</v>
+      </c>
+      <c r="G264" t="n">
+        <v>3.71195387840271</v>
+      </c>
+      <c r="H264" t="n">
+        <v>0.008177928164542776</v>
+      </c>
+      <c r="I264" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J264" t="n">
+        <v>0.0003393011723767292</v>
+      </c>
+      <c r="K264" t="n">
+        <v>40</v>
+      </c>
+      <c r="L264" t="n">
+        <v>64</v>
+      </c>
+      <c r="M264" t="n">
+        <v>128</v>
+      </c>
+      <c r="N264" t="n">
+        <v>128</v>
+      </c>
+      <c r="O264" t="n">
+        <v>32</v>
+      </c>
+      <c r="P264" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q264" t="n">
+        <v>5</v>
+      </c>
+      <c r="R264" t="inlineStr">
+        <is>
+          <t>rmsprop</t>
+        </is>
+      </c>
+      <c r="S264" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T264" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="U264" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="V264" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="W264" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="X264" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>bayesian_optimization</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>50</v>
+      </c>
+      <c r="C265" t="n">
+        <v>6</v>
+      </c>
+      <c r="D265" t="n">
+        <v>36</v>
+      </c>
+      <c r="E265" t="n">
+        <v>0.04697380214929581</v>
+      </c>
+      <c r="F265" t="n">
+        <v>0.04697380214929581</v>
+      </c>
+      <c r="G265" t="n">
+        <v>3.635501861572266</v>
+      </c>
+      <c r="H265" t="n">
+        <v>1.187837283772948e-06</v>
+      </c>
+      <c r="I265" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J265" t="n">
+        <v>0.001555488876314946</v>
+      </c>
+      <c r="K265" t="n">
+        <v>64</v>
+      </c>
+      <c r="L265" t="n">
+        <v>256</v>
+      </c>
+      <c r="M265" t="n">
+        <v>64</v>
+      </c>
+      <c r="N265" t="n">
+        <v>96</v>
+      </c>
+      <c r="O265" t="n">
+        <v>64</v>
+      </c>
+      <c r="P265" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q265" t="n">
+        <v>4</v>
+      </c>
+      <c r="R265" t="inlineStr">
+        <is>
+          <t>rmsprop</t>
+        </is>
+      </c>
+      <c r="S265" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T265" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U265" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V265" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W265" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X265" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>bayesian_optimization</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>50</v>
+      </c>
+      <c r="C266" t="n">
+        <v>6</v>
+      </c>
+      <c r="D266" t="n">
+        <v>47</v>
+      </c>
+      <c r="E266" t="n">
+        <v>0.04607046023011208</v>
+      </c>
+      <c r="F266" t="n">
+        <v>0.04607046023011208</v>
+      </c>
+      <c r="G266" t="n">
+        <v>4.246967315673828</v>
+      </c>
+      <c r="H266" t="n">
+        <v>0.002606060045095223</v>
+      </c>
+      <c r="I266" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="J266" t="n">
+        <v>0.0009969653267339197</v>
+      </c>
+      <c r="K266" t="n">
+        <v>48</v>
+      </c>
+      <c r="L266" t="n">
+        <v>352</v>
+      </c>
+      <c r="M266" t="n">
+        <v>96</v>
+      </c>
+      <c r="N266" t="n">
+        <v>96</v>
+      </c>
+      <c r="O266" t="n">
+        <v>32</v>
+      </c>
+      <c r="P266" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q266" t="n">
+        <v>2</v>
+      </c>
+      <c r="R266" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="S266" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="T266" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="U266" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V266" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W266" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="X266" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>bayesian_optimization</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>50</v>
+      </c>
+      <c r="C267" t="n">
+        <v>6</v>
+      </c>
+      <c r="D267" t="n">
+        <v>177</v>
+      </c>
+      <c r="E267" t="n">
+        <v>0.04516711831092834</v>
+      </c>
+      <c r="F267" t="n">
+        <v>0.04516711831092834</v>
+      </c>
+      <c r="G267" t="n">
+        <v>3.742468118667603</v>
+      </c>
+      <c r="H267" t="n">
+        <v>1.589935843421407e-05</v>
+      </c>
+      <c r="I267" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="J267" t="n">
+        <v>0.0002298877657472638</v>
+      </c>
+      <c r="K267" t="n">
+        <v>56</v>
+      </c>
+      <c r="L267" t="n">
+        <v>384</v>
+      </c>
+      <c r="M267" t="n">
+        <v>192</v>
+      </c>
+      <c r="N267" t="n">
+        <v>64</v>
+      </c>
+      <c r="O267" t="n">
+        <v>32</v>
+      </c>
+      <c r="P267" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q267" t="n">
+        <v>4</v>
+      </c>
+      <c r="R267" t="inlineStr">
+        <is>
+          <t>adamw</t>
+        </is>
+      </c>
+      <c r="S267" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T267" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U267" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="V267" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W267" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="X267" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>bayesian_optimization</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>50</v>
+      </c>
+      <c r="C268" t="n">
+        <v>6</v>
+      </c>
+      <c r="D268" t="n">
+        <v>31</v>
+      </c>
+      <c r="E268" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="F268" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="G268" t="n">
+        <v>3.87192702293396</v>
+      </c>
+      <c r="H268" t="n">
+        <v>2.036784961038523e-05</v>
+      </c>
+      <c r="I268" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="J268" t="n">
+        <v>0.0002288573928398741</v>
+      </c>
+      <c r="K268" t="n">
+        <v>64</v>
+      </c>
+      <c r="L268" t="n">
+        <v>320</v>
+      </c>
+      <c r="M268" t="n">
+        <v>192</v>
+      </c>
+      <c r="N268" t="n">
+        <v>96</v>
+      </c>
+      <c r="O268" t="n">
+        <v>64</v>
+      </c>
+      <c r="P268" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q268" t="n">
+        <v>4</v>
+      </c>
+      <c r="R268" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="S268" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T268" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="U268" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V268" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W268" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X268" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>bayesian_optimization</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>50</v>
+      </c>
+      <c r="C269" t="n">
+        <v>6</v>
+      </c>
+      <c r="D269" t="n">
+        <v>14</v>
+      </c>
+      <c r="E269" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="F269" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="G269" t="n">
+        <v>4.78287410736084</v>
+      </c>
+      <c r="H269" t="n">
+        <v>0.002134326629454137</v>
+      </c>
+      <c r="I269" t="n">
+        <v>0</v>
+      </c>
+      <c r="J269" t="n">
+        <v>3.825916182497886e-05</v>
+      </c>
+      <c r="K269" t="n">
+        <v>16</v>
+      </c>
+      <c r="L269" t="n">
+        <v>128</v>
+      </c>
+      <c r="M269" t="n">
+        <v>128</v>
+      </c>
+      <c r="N269" t="n">
+        <v>64</v>
+      </c>
+      <c r="O269" t="n">
+        <v>64</v>
+      </c>
+      <c r="P269" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q269" t="n">
+        <v>5</v>
+      </c>
+      <c r="R269" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="S269" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T269" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U269" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V269" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W269" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="X269" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>bayesian_optimization</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>50</v>
+      </c>
+      <c r="C270" t="n">
+        <v>6</v>
+      </c>
+      <c r="D270" t="n">
+        <v>49</v>
+      </c>
+      <c r="E270" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="F270" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="G270" t="n">
+        <v>4.164015769958496</v>
+      </c>
+      <c r="H270" t="n">
+        <v>0.005618290609009494</v>
+      </c>
+      <c r="I270" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="J270" t="n">
+        <v>0.0001089554838812193</v>
+      </c>
+      <c r="K270" t="n">
+        <v>64</v>
+      </c>
+      <c r="L270" t="n">
+        <v>256</v>
+      </c>
+      <c r="M270" t="n">
+        <v>32</v>
+      </c>
+      <c r="N270" t="n">
+        <v>64</v>
+      </c>
+      <c r="O270" t="n">
+        <v>64</v>
+      </c>
+      <c r="P270" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q270" t="n">
+        <v>2</v>
+      </c>
+      <c r="R270" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="S270" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="T270" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="U270" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V270" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="W270" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="X270" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>bayesian_optimization</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>50</v>
+      </c>
+      <c r="C271" t="n">
+        <v>6</v>
+      </c>
+      <c r="D271" t="n">
+        <v>51</v>
+      </c>
+      <c r="E271" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="F271" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="G271" t="n">
+        <v>3.648605823516846</v>
+      </c>
+      <c r="H271" t="n">
+        <v>4.665808365764719e-06</v>
+      </c>
+      <c r="I271" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J271" t="n">
+        <v>0.001096043361021397</v>
+      </c>
+      <c r="K271" t="n">
+        <v>64</v>
+      </c>
+      <c r="L271" t="n">
+        <v>288</v>
+      </c>
+      <c r="M271" t="n">
+        <v>128</v>
+      </c>
+      <c r="N271" t="n">
+        <v>96</v>
+      </c>
+      <c r="O271" t="n">
+        <v>64</v>
+      </c>
+      <c r="P271" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q271" t="n">
+        <v>5</v>
+      </c>
+      <c r="R271" t="inlineStr">
+        <is>
+          <t>rmsprop</t>
+        </is>
+      </c>
+      <c r="S271" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T271" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U271" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V271" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W271" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X271" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>bayesian_optimization</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>50</v>
+      </c>
+      <c r="C272" t="n">
+        <v>6</v>
+      </c>
+      <c r="D272" t="n">
+        <v>145</v>
+      </c>
+      <c r="E272" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="F272" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="G272" t="n">
+        <v>3.669873952865601</v>
+      </c>
+      <c r="H272" t="n">
+        <v>1.420422995169136e-06</v>
+      </c>
+      <c r="I272" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="J272" t="n">
+        <v>0.001523691660962668</v>
+      </c>
+      <c r="K272" t="n">
+        <v>24</v>
+      </c>
+      <c r="L272" t="n">
+        <v>512</v>
+      </c>
+      <c r="M272" t="n">
+        <v>128</v>
+      </c>
+      <c r="N272" t="n">
+        <v>128</v>
+      </c>
+      <c r="O272" t="n">
+        <v>32</v>
+      </c>
+      <c r="P272" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q272" t="n">
+        <v>3</v>
+      </c>
+      <c r="R272" t="inlineStr">
+        <is>
+          <t>adamw</t>
+        </is>
+      </c>
+      <c r="S272" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T272" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U272" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V272" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="W272" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X272" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>random_search</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>50</v>
+      </c>
+      <c r="C273" t="n">
+        <v>6</v>
+      </c>
+      <c r="D273" t="inlineStr">
+        <is>
+          <t>050</t>
+        </is>
+      </c>
+      <c r="E273" t="n">
+        <v>0.04878048598766327</v>
+      </c>
+      <c r="F273" t="n">
+        <v>0.04878048598766327</v>
+      </c>
+      <c r="G273" t="n">
+        <v>4.24997615814209</v>
+      </c>
+      <c r="H273" t="n">
+        <v>0.002976769475342372</v>
+      </c>
+      <c r="I273" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="J273" t="n">
+        <v>0.0005696691651650657</v>
+      </c>
+      <c r="K273" t="n">
+        <v>64</v>
+      </c>
+      <c r="L273" t="n">
+        <v>160</v>
+      </c>
+      <c r="M273" t="n">
+        <v>96</v>
+      </c>
+      <c r="N273" t="n">
+        <v>96</v>
+      </c>
+      <c r="O273" t="n">
+        <v>64</v>
+      </c>
+      <c r="P273" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q273" t="n">
+        <v>3</v>
+      </c>
+      <c r="R273" t="inlineStr">
+        <is>
+          <t>adamw</t>
+        </is>
+      </c>
+      <c r="S273" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T273" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="U273" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V273" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="W273" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X273" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>random_search</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>50</v>
+      </c>
+      <c r="C274" t="n">
+        <v>6</v>
+      </c>
+      <c r="D274" t="inlineStr">
+        <is>
+          <t>157</t>
+        </is>
+      </c>
+      <c r="E274" t="n">
+        <v>0.04878048598766327</v>
+      </c>
+      <c r="F274" t="n">
+        <v>0.04878048598766327</v>
+      </c>
+      <c r="G274" t="n">
+        <v>4.383533954620361</v>
+      </c>
+      <c r="H274" t="n">
+        <v>0.009306905006616356</v>
+      </c>
+      <c r="I274" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="J274" t="n">
+        <v>0.0001786009552267408</v>
+      </c>
+      <c r="K274" t="n">
+        <v>40</v>
+      </c>
+      <c r="L274" t="n">
+        <v>224</v>
+      </c>
+      <c r="M274" t="n">
+        <v>128</v>
+      </c>
+      <c r="N274" t="n">
+        <v>32</v>
+      </c>
+      <c r="O274" t="n">
+        <v>64</v>
+      </c>
+      <c r="P274" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q274" t="n">
+        <v>5</v>
+      </c>
+      <c r="R274" t="inlineStr">
+        <is>
+          <t>rmsprop</t>
+        </is>
+      </c>
+      <c r="S274" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T274" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U274" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V274" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="W274" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X274" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>random_search</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>50</v>
+      </c>
+      <c r="C275" t="n">
+        <v>6</v>
+      </c>
+      <c r="D275" t="inlineStr">
+        <is>
+          <t>262</t>
+        </is>
+      </c>
+      <c r="E275" t="n">
+        <v>0.04697380214929581</v>
+      </c>
+      <c r="F275" t="n">
+        <v>0.04697380214929581</v>
+      </c>
+      <c r="G275" t="n">
+        <v>4.013683319091797</v>
+      </c>
+      <c r="H275" t="n">
+        <v>0.001406145697905212</v>
+      </c>
+      <c r="I275" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="J275" t="n">
+        <v>5.037984701372031e-05</v>
+      </c>
+      <c r="K275" t="n">
+        <v>8</v>
+      </c>
+      <c r="L275" t="n">
+        <v>384</v>
+      </c>
+      <c r="M275" t="n">
+        <v>192</v>
+      </c>
+      <c r="N275" t="n">
+        <v>32</v>
+      </c>
+      <c r="O275" t="n">
+        <v>64</v>
+      </c>
+      <c r="P275" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q275" t="n">
+        <v>2</v>
+      </c>
+      <c r="R275" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="S275" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="T275" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="U275" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="V275" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W275" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="X275" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>random_search</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>50</v>
+      </c>
+      <c r="C276" t="n">
+        <v>6</v>
+      </c>
+      <c r="D276" t="inlineStr">
+        <is>
+          <t>227</t>
+        </is>
+      </c>
+      <c r="E276" t="n">
+        <v>0.04607046023011208</v>
+      </c>
+      <c r="F276" t="n">
+        <v>0.04607046023011208</v>
+      </c>
+      <c r="G276" t="n">
+        <v>4.26451301574707</v>
+      </c>
+      <c r="H276" t="n">
+        <v>0.0005772563072289049</v>
+      </c>
+      <c r="I276" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="J276" t="n">
+        <v>0.0005392665987313878</v>
+      </c>
+      <c r="K276" t="n">
+        <v>56</v>
+      </c>
+      <c r="L276" t="n">
+        <v>480</v>
+      </c>
+      <c r="M276" t="n">
+        <v>160</v>
+      </c>
+      <c r="N276" t="n">
+        <v>128</v>
+      </c>
+      <c r="O276" t="n">
+        <v>32</v>
+      </c>
+      <c r="P276" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q276" t="n">
+        <v>2</v>
+      </c>
+      <c r="R276" t="inlineStr">
+        <is>
+          <t>adamw</t>
+        </is>
+      </c>
+      <c r="S276" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="T276" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="U276" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V276" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="W276" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X276" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>random_search</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>50</v>
+      </c>
+      <c r="C277" t="n">
+        <v>6</v>
+      </c>
+      <c r="D277" t="inlineStr">
+        <is>
+          <t>048</t>
+        </is>
+      </c>
+      <c r="E277" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="F277" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="G277" t="n">
+        <v>3.694175720214844</v>
+      </c>
+      <c r="H277" t="n">
+        <v>1.098738598331986e-06</v>
+      </c>
+      <c r="I277" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J277" t="n">
+        <v>0.0001926517007245992</v>
+      </c>
+      <c r="K277" t="n">
+        <v>56</v>
+      </c>
+      <c r="L277" t="n">
+        <v>160</v>
+      </c>
+      <c r="M277" t="n">
+        <v>32</v>
+      </c>
+      <c r="N277" t="n">
+        <v>96</v>
+      </c>
+      <c r="O277" t="n">
+        <v>64</v>
+      </c>
+      <c r="P277" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q277" t="n">
+        <v>3</v>
+      </c>
+      <c r="R277" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="S277" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T277" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="U277" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V277" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W277" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X277" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>random_search</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>50</v>
+      </c>
+      <c r="C278" t="n">
+        <v>6</v>
+      </c>
+      <c r="D278" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="E278" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="F278" t="n">
+        <v>0.04426377639174461</v>
+      </c>
+      <c r="G278" t="n">
+        <v>3.647773742675781</v>
+      </c>
+      <c r="H278" t="n">
+        <v>5.167629476613872e-05</v>
+      </c>
+      <c r="I278" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="J278" t="n">
+        <v>0.003559569044117667</v>
+      </c>
+      <c r="K278" t="n">
+        <v>32</v>
+      </c>
+      <c r="L278" t="n">
+        <v>448</v>
+      </c>
+      <c r="M278" t="n">
+        <v>128</v>
+      </c>
+      <c r="N278" t="n">
+        <v>128</v>
+      </c>
+      <c r="O278" t="n">
+        <v>32</v>
+      </c>
+      <c r="P278" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q278" t="n">
+        <v>3</v>
+      </c>
+      <c r="R278" t="inlineStr">
+        <is>
+          <t>rmsprop</t>
+        </is>
+      </c>
+      <c r="S278" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="T278" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U278" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V278" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W278" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X278" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>random_search</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>50</v>
+      </c>
+      <c r="C279" t="n">
+        <v>6</v>
+      </c>
+      <c r="D279" t="inlineStr">
+        <is>
+          <t>051</t>
+        </is>
+      </c>
+      <c r="E279" t="n">
+        <v>0.04336043447256088</v>
+      </c>
+      <c r="F279" t="n">
+        <v>0.04336043447256088</v>
+      </c>
+      <c r="G279" t="n">
+        <v>3.948803186416626</v>
+      </c>
+      <c r="H279" t="n">
+        <v>0.009737742886304799</v>
+      </c>
+      <c r="I279" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J279" t="n">
+        <v>0.0001015972175793971</v>
+      </c>
+      <c r="K279" t="n">
+        <v>8</v>
+      </c>
+      <c r="L279" t="n">
+        <v>160</v>
+      </c>
+      <c r="M279" t="n">
+        <v>160</v>
+      </c>
+      <c r="N279" t="n">
+        <v>96</v>
+      </c>
+      <c r="O279" t="n">
+        <v>32</v>
+      </c>
+      <c r="P279" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q279" t="n">
+        <v>3</v>
+      </c>
+      <c r="R279" t="inlineStr">
+        <is>
+          <t>rmsprop</t>
+        </is>
+      </c>
+      <c r="S279" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T279" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="U279" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="V279" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W279" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X279" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>random_search</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>50</v>
+      </c>
+      <c r="C280" t="n">
+        <v>6</v>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>127</t>
+        </is>
+      </c>
+      <c r="E280" t="n">
+        <v>0.04336043447256088</v>
+      </c>
+      <c r="F280" t="n">
+        <v>0.04336043447256088</v>
+      </c>
+      <c r="G280" t="n">
+        <v>3.862306118011475</v>
+      </c>
+      <c r="H280" t="n">
+        <v>0.0003695776045851694</v>
+      </c>
+      <c r="I280" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="J280" t="n">
+        <v>0.0002876054398079882</v>
+      </c>
+      <c r="K280" t="n">
+        <v>32</v>
+      </c>
+      <c r="L280" t="n">
+        <v>96</v>
+      </c>
+      <c r="M280" t="n">
+        <v>64</v>
+      </c>
+      <c r="N280" t="n">
+        <v>96</v>
+      </c>
+      <c r="O280" t="n">
+        <v>64</v>
+      </c>
+      <c r="P280" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q280" t="n">
+        <v>3</v>
+      </c>
+      <c r="R280" t="inlineStr">
+        <is>
+          <t>rmsprop</t>
+        </is>
+      </c>
+      <c r="S280" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T280" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U280" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V280" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="W280" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="X280" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>random_search</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>50</v>
+      </c>
+      <c r="C281" t="n">
+        <v>6</v>
+      </c>
+      <c r="D281" t="inlineStr">
+        <is>
+          <t>203</t>
+        </is>
+      </c>
+      <c r="E281" t="n">
+        <v>0.04336043447256088</v>
+      </c>
+      <c r="F281" t="n">
+        <v>0.04336043447256088</v>
+      </c>
+      <c r="G281" t="n">
+        <v>4.49708890914917</v>
+      </c>
+      <c r="H281" t="n">
+        <v>0.003692347622649561</v>
+      </c>
+      <c r="I281" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="J281" t="n">
+        <v>0.0002899736467359285</v>
+      </c>
+      <c r="K281" t="n">
+        <v>16</v>
+      </c>
+      <c r="L281" t="n">
+        <v>128</v>
+      </c>
+      <c r="M281" t="n">
+        <v>96</v>
+      </c>
+      <c r="N281" t="n">
+        <v>96</v>
+      </c>
+      <c r="O281" t="n">
+        <v>64</v>
+      </c>
+      <c r="P281" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q281" t="n">
+        <v>5</v>
+      </c>
+      <c r="R281" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="S281" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="T281" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U281" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V281" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="W281" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="X281" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>random_search</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>50</v>
+      </c>
+      <c r="C282" t="n">
+        <v>6</v>
+      </c>
+      <c r="D282" t="inlineStr">
+        <is>
+          <t>017</t>
+        </is>
+      </c>
+      <c r="E282" t="n">
+        <v>0.04245709255337715</v>
+      </c>
+      <c r="F282" t="n">
+        <v>0.04245709255337715</v>
+      </c>
+      <c r="G282" t="n">
+        <v>3.612314701080322</v>
+      </c>
+      <c r="H282" t="n">
+        <v>1.50258421960589e-05</v>
+      </c>
+      <c r="I282" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="J282" t="n">
+        <v>0.0004846497851843258</v>
+      </c>
+      <c r="K282" t="n">
+        <v>24</v>
+      </c>
+      <c r="L282" t="n">
+        <v>32</v>
+      </c>
+      <c r="M282" t="n">
+        <v>128</v>
+      </c>
+      <c r="N282" t="n">
+        <v>96</v>
+      </c>
+      <c r="O282" t="n">
+        <v>32</v>
+      </c>
+      <c r="P282" t="n">
+        <v>32</v>
+      </c>
+      <c r="Q282" t="n">
+        <v>2</v>
+      </c>
+      <c r="R282" t="inlineStr">
+        <is>
+          <t>adam</t>
+        </is>
+      </c>
+      <c r="S282" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="T282" t="inlineStr">
+        <is>
+          <t>GRU</t>
+        </is>
+      </c>
+      <c r="U282" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="V282" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="W282" t="inlineStr">
+        <is>
+          <t>LSTM</t>
+        </is>
+      </c>
+      <c r="X282" t="n">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>